<commit_message>
Added an expander to hide the filter options if needed, also added filter options for sound type, probabilty and date.
</commit_message>
<xml_diff>
--- a/prototype/eventmapdata.xlsx
+++ b/prototype/eventmapdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Groep1ProjectD\prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0A91F8-C4A9-4C42-8AF4-BC358879C781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F725C-1EFE-412A-B9B3-9107D45F7853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="5775" windowWidth="23730" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2790" windowWidth="23730" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>time</t>
   </si>
@@ -48,22 +48,16 @@
     <t>sound</t>
   </si>
   <si>
-    <t>"1648804145"</t>
-  </si>
-  <si>
-    <t>"1648804146"</t>
-  </si>
-  <si>
-    <t>"gun"</t>
-  </si>
-  <si>
-    <t>"car"</t>
-  </si>
-  <si>
     <t>http://95.217.2.100:8000/124489-9-0-12.wav</t>
   </si>
   <si>
-    <t>"animal"</t>
+    <t>gun</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>animal</t>
   </si>
 </sst>
 </file>
@@ -395,7 +389,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +398,7 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -434,8 +429,8 @@
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>1648804145</v>
       </c>
       <c r="C2">
         <v>22.67591028153668</v>
@@ -444,21 +439,21 @@
         <v>5.3372457867986762</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3">
+        <v>1648804146</v>
       </c>
       <c r="C3">
         <v>-2.4271979847212402</v>
@@ -467,21 +462,21 @@
         <v>23.192179136569301</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>95</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4">
+        <v>1648804146</v>
       </c>
       <c r="C4">
         <v>-2.1831842689999998</v>
@@ -490,13 +485,13 @@
         <v>23.520216261000002</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>